<commit_message>
tmp: master story data
</commit_message>
<xml_diff>
--- a/master_story.xlsx
+++ b/master_story.xlsx
@@ -6,7 +6,7 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="01_02 - 表 1" sheetId="1" r:id="rId4"/>
+    <sheet name="01_02" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -90,7 +90,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -102,9 +102,14 @@
       <name val="ヒラギノ角ゴ ProN W3"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="ヒラギノ角ゴ ProN W3"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
     </font>
     <font>
       <sz val="10"/>
@@ -112,8 +117,13 @@
       <name val="ヒラギノ角ゴ ProN W6"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="ヒラギノ角ゴ ProN W3"/>
+    </font>
+    <font>
       <sz val="14"/>
-      <color indexed="11"/>
+      <color indexed="12"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -126,21 +136,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
+        <fgColor indexed="10"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -160,35 +216,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -208,6 +292,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ff3c4a60"/>
@@ -1442,235 +1527,252 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:F19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="C1" xSplit="2" ySplit="0" activePane="topRight" state="frozenSplit"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="23" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="12.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="83.1953" style="1" customWidth="1"/>
+    <col min="3" max="3" width="83.25" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.25" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.25" style="1" customWidth="1"/>
     <col min="7" max="256" width="12.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" t="s" s="2">
+    <row r="1" ht="23" customHeight="1">
+      <c r="A1" s="2"/>
+      <c r="B1" t="s" s="3">
         <v>0</v>
       </c>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
-      <c r="F1"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" ht="18.5" customHeight="1">
-      <c r="B2" t="s" s="3">
+      <c r="A2" s="6"/>
+      <c r="B2" t="s" s="7">
         <v>1</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="7">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="7">
         <v>3</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" t="s" s="7">
         <v>4</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" t="s" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="3" ht="23.55" customHeight="1">
-      <c r="B3" s="4">
+      <c r="A3" s="6"/>
+      <c r="B3" s="8">
         <v>1</v>
       </c>
-      <c r="C3" t="s" s="5">
+      <c r="C3" t="s" s="9">
         <v>6</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" ht="23.35" customHeight="1">
-      <c r="B4" s="4">
+      <c r="A4" s="6"/>
+      <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C4" t="s" s="5">
+      <c r="C4" t="s" s="9">
         <v>7</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" ht="23.35" customHeight="1">
-      <c r="B5" s="4">
+      <c r="A5" s="6"/>
+      <c r="B5" s="8">
         <v>1</v>
       </c>
-      <c r="C5" t="s" s="5">
+      <c r="C5" t="s" s="9">
         <v>8</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" ht="23.35" customHeight="1">
-      <c r="B6" s="4">
+      <c r="A6" s="6"/>
+      <c r="B6" s="8">
         <v>1</v>
       </c>
-      <c r="C6" t="s" s="7">
+      <c r="C6" t="s" s="11">
         <v>9</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" ht="23.35" customHeight="1">
-      <c r="B7" s="4">
+      <c r="A7" s="6"/>
+      <c r="B7" s="8">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="7">
+      <c r="C7" t="s" s="11">
         <v>10</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" ht="23.35" customHeight="1">
-      <c r="B8" s="4">
+      <c r="A8" s="6"/>
+      <c r="B8" s="8">
         <v>1</v>
       </c>
-      <c r="C8" t="s" s="7">
+      <c r="C8" t="s" s="11">
         <v>11</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
     </row>
     <row r="9" ht="23.35" customHeight="1">
-      <c r="B9" s="4">
+      <c r="A9" s="6"/>
+      <c r="B9" s="8">
         <v>1</v>
       </c>
-      <c r="C9" t="s" s="7">
+      <c r="C9" t="s" s="11">
         <v>12</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" ht="23.35" customHeight="1">
-      <c r="B10" s="4">
+      <c r="A10" s="6"/>
+      <c r="B10" s="8">
         <v>1</v>
       </c>
-      <c r="C10" t="s" s="7">
+      <c r="C10" t="s" s="11">
         <v>13</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" ht="23.85" customHeight="1">
-      <c r="B11" s="4">
+      <c r="A11" s="6"/>
+      <c r="B11" s="8">
         <v>1</v>
       </c>
-      <c r="C11" t="s" s="7">
+      <c r="C11" t="s" s="11">
         <v>14</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" ht="23.85" customHeight="1">
-      <c r="B12" s="4">
+      <c r="A12" s="6"/>
+      <c r="B12" s="8">
         <v>1</v>
       </c>
-      <c r="C12" t="s" s="7">
+      <c r="C12" t="s" s="11">
         <v>15</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" ht="23.35" customHeight="1">
-      <c r="B13" s="4">
+      <c r="A13" s="6"/>
+      <c r="B13" s="8">
         <v>1</v>
       </c>
-      <c r="C13" t="s" s="7">
+      <c r="C13" t="s" s="11">
         <v>16</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
     </row>
     <row r="14" ht="23.35" customHeight="1">
-      <c r="B14" s="4">
+      <c r="A14" s="6"/>
+      <c r="B14" s="8">
         <v>1</v>
       </c>
-      <c r="C14" t="s" s="7">
+      <c r="C14" t="s" s="11">
         <v>17</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
     </row>
     <row r="15" ht="23.35" customHeight="1">
-      <c r="B15" s="4">
+      <c r="A15" s="6"/>
+      <c r="B15" s="8">
         <v>1</v>
       </c>
-      <c r="C15" t="s" s="7">
+      <c r="C15" t="s" s="11">
         <v>18</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
     </row>
     <row r="16" ht="23.35" customHeight="1">
-      <c r="B16" s="4">
+      <c r="A16" s="6"/>
+      <c r="B16" s="8">
         <v>1</v>
       </c>
-      <c r="C16" t="s" s="7">
+      <c r="C16" t="s" s="11">
         <v>19</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
     </row>
     <row r="17" ht="23.35" customHeight="1">
-      <c r="B17" s="4">
+      <c r="A17" s="6"/>
+      <c r="B17" s="8">
         <v>1</v>
       </c>
-      <c r="C17" t="s" s="7">
+      <c r="C17" t="s" s="11">
         <v>20</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
     </row>
     <row r="18" ht="23.35" customHeight="1">
-      <c r="B18" s="4">
+      <c r="A18" s="6"/>
+      <c r="B18" s="8">
         <v>1</v>
       </c>
-      <c r="C18" t="s" s="7">
+      <c r="C18" t="s" s="11">
         <v>21</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
     </row>
     <row r="19" ht="23.85" customHeight="1">
-      <c r="B19" s="4">
+      <c r="A19" s="12"/>
+      <c r="B19" s="8">
         <v>1</v>
       </c>
-      <c r="C19" t="s" s="7">
+      <c r="C19" t="s" s="11">
         <v>22</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>